<commit_message>
Final commit before submission, renamed a bunch of files.
</commit_message>
<xml_diff>
--- a/hw3/DataDictionary.xlsx
+++ b/hw3/DataDictionary.xlsx
@@ -708,10 +708,17 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F41"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22">
       <c r="A1" s="1" t="s">
@@ -1261,16 +1268,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:B26"/>
+    <mergeCell ref="C20:C26"/>
+    <mergeCell ref="D20:D26"/>
+    <mergeCell ref="E20:E26"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="E17:E19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:B26"/>
-    <mergeCell ref="C20:C26"/>
-    <mergeCell ref="D20:D26"/>
-    <mergeCell ref="E20:E26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F14" r:id="rId1"/>

</xml_diff>